<commit_message>
unified data frame created.
</commit_message>
<xml_diff>
--- a/content/data_dictionary.xlsx
+++ b/content/data_dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pdoyle/school/capstone/content/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC496A25-8ABF-464C-9CBF-6B26D2A96912}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A630768-5541-3142-9DBB-8DE1EF2EFFED}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1940" yWindow="4860" windowWidth="22360" windowHeight="36480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="320" yWindow="460" windowWidth="16340" windowHeight="19140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Fundamentals" sheetId="2" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4258" uniqueCount="3681">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4280" uniqueCount="3687">
   <si>
     <t>gvkey</t>
   </si>
@@ -11074,6 +11074,24 @@
   </si>
   <si>
     <t>cat</t>
+  </si>
+  <si>
+    <t>use</t>
+  </si>
+  <si>
+    <t>STD</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>agg to year</t>
+  </si>
+  <si>
+    <t>agg to month then to year</t>
+  </si>
+  <si>
+    <t>change to integer and agg to per year</t>
   </si>
 </sst>
 </file>
@@ -11403,10 +11421,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:E1769"/>
+  <dimension ref="A1:F1769"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A544" zoomScale="172" zoomScaleNormal="172" workbookViewId="0">
-      <selection activeCell="D623" sqref="D623"/>
+    <sheetView tabSelected="1" topLeftCell="A754" zoomScale="123" zoomScaleNormal="123" workbookViewId="0">
+      <selection activeCell="C777" sqref="C777"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11415,7 +11433,7 @@
     <col min="2" max="2" width="55.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>3588</v>
       </c>
@@ -11431,8 +11449,11 @@
       <c r="E1" t="s">
         <v>3679</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" t="s">
+        <v>3681</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -11445,8 +11466,11 @@
       <c r="D2" t="s">
         <v>3673</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -11459,8 +11483,11 @@
       <c r="D3" t="s">
         <v>3674</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>151</v>
       </c>
@@ -11473,8 +11500,11 @@
       <c r="D4" t="s">
         <v>3675</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="F4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>152</v>
       </c>
@@ -11485,7 +11515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>153</v>
       </c>
@@ -11496,7 +11526,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>154</v>
       </c>
@@ -11507,7 +11537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>155</v>
       </c>
@@ -11520,8 +11550,11 @@
       <c r="D8" t="s">
         <v>3676</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F8" t="s">
+        <v>3682</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -11534,8 +11567,11 @@
       <c r="D9" t="s">
         <v>3677</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -11548,8 +11584,11 @@
       <c r="D10" t="s">
         <v>3677</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>156</v>
       </c>
@@ -11557,13 +11596,16 @@
         <v>1885</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D11" t="s">
         <v>3677</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="F11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>157</v>
       </c>
@@ -11574,7 +11616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>158</v>
       </c>
@@ -11585,7 +11627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>159</v>
       </c>
@@ -11596,7 +11638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>160</v>
       </c>
@@ -11610,7 +11652,7 @@
         <v>3678</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>161</v>
       </c>
@@ -11618,7 +11660,7 @@
         <v>1890</v>
       </c>
       <c r="C16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D16" t="s">
         <v>3678</v>
@@ -11657,7 +11699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>165</v>
       </c>
@@ -11665,7 +11707,7 @@
         <v>1894</v>
       </c>
       <c r="C20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D20" t="s">
         <v>3677</v>
@@ -11707,7 +11749,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>169</v>
       </c>
@@ -11715,7 +11757,7 @@
         <v>1898</v>
       </c>
       <c r="C24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D24" t="s">
         <v>3673</v>
@@ -11886,7 +11928,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>185</v>
       </c>
@@ -11894,10 +11936,13 @@
         <v>1914</v>
       </c>
       <c r="C40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="D40" t="s">
+        <v>3678</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>186</v>
       </c>
@@ -11905,7 +11950,7 @@
         <v>1915</v>
       </c>
       <c r="C41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D41" t="s">
         <v>3678</v>
@@ -11983,7 +12028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>193</v>
       </c>
@@ -11991,13 +12036,13 @@
         <v>1922</v>
       </c>
       <c r="C48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D48" t="s">
         <v>3678</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>194</v>
       </c>
@@ -12005,13 +12050,13 @@
         <v>1923</v>
       </c>
       <c r="C49">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D49" t="s">
         <v>3678</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>195</v>
       </c>
@@ -12019,7 +12064,7 @@
         <v>1924</v>
       </c>
       <c r="C50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D50" t="s">
         <v>3678</v>
@@ -12047,7 +12092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>198</v>
       </c>
@@ -12055,13 +12100,13 @@
         <v>1927</v>
       </c>
       <c r="C53">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D53" t="s">
         <v>3678</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>199</v>
       </c>
@@ -12069,7 +12114,7 @@
         <v>1928</v>
       </c>
       <c r="C54">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D54" t="s">
         <v>3678</v>
@@ -12133,7 +12178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>205</v>
       </c>
@@ -12141,7 +12186,7 @@
         <v>1934</v>
       </c>
       <c r="C60">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D60" t="s">
         <v>3678</v>
@@ -12395,7 +12440,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>225</v>
       </c>
@@ -12403,7 +12448,7 @@
         <v>1954</v>
       </c>
       <c r="C80">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D80" t="s">
         <v>3678</v>
@@ -12423,7 +12468,7 @@
         <v>3678</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>227</v>
       </c>
@@ -12431,13 +12476,13 @@
         <v>1956</v>
       </c>
       <c r="C82">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D82" t="s">
         <v>3678</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>228</v>
       </c>
@@ -12445,13 +12490,13 @@
         <v>1957</v>
       </c>
       <c r="C83">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D83" t="s">
         <v>3678</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>229</v>
       </c>
@@ -12459,13 +12504,13 @@
         <v>1958</v>
       </c>
       <c r="C84">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D84" t="s">
         <v>3678</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>230</v>
       </c>
@@ -12473,7 +12518,7 @@
         <v>1959</v>
       </c>
       <c r="C85">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D85" t="s">
         <v>3678</v>
@@ -12493,7 +12538,7 @@
         <v>3678</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>232</v>
       </c>
@@ -12501,7 +12546,7 @@
         <v>1961</v>
       </c>
       <c r="C87">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D87" t="s">
         <v>3678</v>
@@ -12634,7 +12679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>244</v>
       </c>
@@ -12642,13 +12687,13 @@
         <v>1973</v>
       </c>
       <c r="C99">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D99" t="s">
         <v>3678</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>245</v>
       </c>
@@ -12656,7 +12701,7 @@
         <v>1974</v>
       </c>
       <c r="C100">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D100" t="s">
         <v>3678</v>
@@ -14411,7 +14456,7 @@
         <v>3678</v>
       </c>
     </row>
-    <row r="242" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
         <v>387</v>
       </c>
@@ -14419,13 +14464,13 @@
         <v>2116</v>
       </c>
       <c r="C242">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D242" t="s">
         <v>3678</v>
       </c>
     </row>
-    <row r="243" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
         <v>388</v>
       </c>
@@ -14433,13 +14478,13 @@
         <v>2117</v>
       </c>
       <c r="C243">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D243" t="s">
         <v>3678</v>
       </c>
     </row>
-    <row r="244" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
         <v>389</v>
       </c>
@@ -14447,13 +14492,13 @@
         <v>2118</v>
       </c>
       <c r="C244">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D244" t="s">
         <v>3678</v>
       </c>
     </row>
-    <row r="245" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
         <v>390</v>
       </c>
@@ -14461,7 +14506,7 @@
         <v>2119</v>
       </c>
       <c r="C245">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D245" t="s">
         <v>3678</v>
@@ -15248,7 +15293,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="308" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A308" t="s">
         <v>453</v>
       </c>
@@ -15256,13 +15301,13 @@
         <v>2182</v>
       </c>
       <c r="C308">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D308" t="s">
         <v>3678</v>
       </c>
     </row>
-    <row r="309" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A309" t="s">
         <v>454</v>
       </c>
@@ -15270,13 +15315,13 @@
         <v>2183</v>
       </c>
       <c r="C309">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D309" t="s">
         <v>3678</v>
       </c>
     </row>
-    <row r="310" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A310" t="s">
         <v>455</v>
       </c>
@@ -15284,13 +15329,13 @@
         <v>2184</v>
       </c>
       <c r="C310">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D310" t="s">
         <v>3678</v>
       </c>
     </row>
-    <row r="311" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A311" t="s">
         <v>456</v>
       </c>
@@ -15298,7 +15343,7 @@
         <v>2185</v>
       </c>
       <c r="C311">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D311" t="s">
         <v>3678</v>
@@ -15315,7 +15360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="313" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A313" t="s">
         <v>458</v>
       </c>
@@ -15323,13 +15368,13 @@
         <v>2187</v>
       </c>
       <c r="C313">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D313" t="s">
         <v>3678</v>
       </c>
     </row>
-    <row r="314" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A314" t="s">
         <v>459</v>
       </c>
@@ -15337,13 +15382,13 @@
         <v>2188</v>
       </c>
       <c r="C314">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D314" t="s">
         <v>3678</v>
       </c>
     </row>
-    <row r="315" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A315" t="s">
         <v>460</v>
       </c>
@@ -15351,13 +15396,13 @@
         <v>2189</v>
       </c>
       <c r="C315">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D315" t="s">
         <v>3678</v>
       </c>
     </row>
-    <row r="316" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A316" t="s">
         <v>461</v>
       </c>
@@ -15365,13 +15410,13 @@
         <v>2190</v>
       </c>
       <c r="C316">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D316" t="s">
         <v>3678</v>
       </c>
     </row>
-    <row r="317" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A317" t="s">
         <v>462</v>
       </c>
@@ -15379,13 +15424,13 @@
         <v>2191</v>
       </c>
       <c r="C317">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D317" t="s">
         <v>3678</v>
       </c>
     </row>
-    <row r="318" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A318" t="s">
         <v>463</v>
       </c>
@@ -15393,13 +15438,13 @@
         <v>2192</v>
       </c>
       <c r="C318">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D318" t="s">
         <v>3678</v>
       </c>
     </row>
-    <row r="319" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A319" t="s">
         <v>464</v>
       </c>
@@ -15407,13 +15452,13 @@
         <v>2193</v>
       </c>
       <c r="C319">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D319" t="s">
         <v>3678</v>
       </c>
     </row>
-    <row r="320" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A320" t="s">
         <v>465</v>
       </c>
@@ -15421,7 +15466,7 @@
         <v>2194</v>
       </c>
       <c r="C320">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D320" t="s">
         <v>3678</v>
@@ -15529,7 +15574,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="330" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="330" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A330" t="s">
         <v>475</v>
       </c>
@@ -15537,7 +15582,7 @@
         <v>2204</v>
       </c>
       <c r="C330">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D330" t="s">
         <v>3678</v>
@@ -16309,7 +16354,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="396" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="396" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A396" t="s">
         <v>541</v>
       </c>
@@ -16317,7 +16362,7 @@
         <v>2270</v>
       </c>
       <c r="C396">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D396" t="s">
         <v>3678</v>
@@ -17597,7 +17642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="503" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="503" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A503" t="s">
         <v>648</v>
       </c>
@@ -17605,13 +17650,13 @@
         <v>2377</v>
       </c>
       <c r="C503">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D503" t="s">
         <v>3678</v>
       </c>
     </row>
-    <row r="504" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="504" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A504" t="s">
         <v>649</v>
       </c>
@@ -17619,7 +17664,7 @@
         <v>2378</v>
       </c>
       <c r="C504">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D504" t="s">
         <v>3678</v>
@@ -17744,7 +17789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="515" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="515" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A515" t="s">
         <v>660</v>
       </c>
@@ -17752,13 +17797,13 @@
         <v>2389</v>
       </c>
       <c r="C515">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D515" t="s">
         <v>3678</v>
       </c>
     </row>
-    <row r="516" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="516" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A516" t="s">
         <v>661</v>
       </c>
@@ -17766,7 +17811,7 @@
         <v>2390</v>
       </c>
       <c r="C516">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D516" t="s">
         <v>3678</v>
@@ -18354,7 +18399,7 @@
         <v>3678</v>
       </c>
     </row>
-    <row r="562" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="562" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A562" t="s">
         <v>707</v>
       </c>
@@ -18362,13 +18407,13 @@
         <v>2436</v>
       </c>
       <c r="C562">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D562" t="s">
         <v>3678</v>
       </c>
     </row>
-    <row r="563" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="563" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A563" t="s">
         <v>708</v>
       </c>
@@ -18376,13 +18421,13 @@
         <v>2437</v>
       </c>
       <c r="C563">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D563" t="s">
         <v>3678</v>
       </c>
     </row>
-    <row r="564" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="564" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A564" t="s">
         <v>709</v>
       </c>
@@ -18390,13 +18435,13 @@
         <v>2438</v>
       </c>
       <c r="C564">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D564" t="s">
         <v>3678</v>
       </c>
     </row>
-    <row r="565" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="565" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A565" t="s">
         <v>710</v>
       </c>
@@ -18404,13 +18449,13 @@
         <v>2439</v>
       </c>
       <c r="C565">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D565" t="s">
         <v>3678</v>
       </c>
     </row>
-    <row r="566" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="566" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A566" t="s">
         <v>711</v>
       </c>
@@ -18418,13 +18463,13 @@
         <v>2440</v>
       </c>
       <c r="C566">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D566" t="s">
         <v>3678</v>
       </c>
     </row>
-    <row r="567" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="567" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A567" t="s">
         <v>712</v>
       </c>
@@ -18432,13 +18477,13 @@
         <v>2441</v>
       </c>
       <c r="C567">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D567" t="s">
         <v>3678</v>
       </c>
     </row>
-    <row r="568" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="568" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A568" t="s">
         <v>713</v>
       </c>
@@ -18446,13 +18491,13 @@
         <v>2442</v>
       </c>
       <c r="C568">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D568" t="s">
         <v>3678</v>
       </c>
     </row>
-    <row r="569" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="569" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A569" t="s">
         <v>714</v>
       </c>
@@ -18460,7 +18505,7 @@
         <v>2443</v>
       </c>
       <c r="C569">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D569" t="s">
         <v>3678</v>
@@ -19083,7 +19128,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="622" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="622" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A622" t="s">
         <v>767</v>
       </c>
@@ -19091,13 +19136,13 @@
         <v>2496</v>
       </c>
       <c r="C622">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D622" t="s">
         <v>3678</v>
       </c>
     </row>
-    <row r="623" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="623" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A623" t="s">
         <v>768</v>
       </c>
@@ -19105,13 +19150,13 @@
         <v>2497</v>
       </c>
       <c r="C623">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D623" t="s">
         <v>3678</v>
       </c>
     </row>
-    <row r="624" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="624" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A624" t="s">
         <v>769</v>
       </c>
@@ -19119,13 +19164,13 @@
         <v>2498</v>
       </c>
       <c r="C624">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D624" t="s">
         <v>3678</v>
       </c>
     </row>
-    <row r="625" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="625" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A625" t="s">
         <v>770</v>
       </c>
@@ -19133,13 +19178,13 @@
         <v>2499</v>
       </c>
       <c r="C625">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D625" t="s">
         <v>3678</v>
       </c>
     </row>
-    <row r="626" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="626" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A626" t="s">
         <v>771</v>
       </c>
@@ -19147,7 +19192,7 @@
         <v>2500</v>
       </c>
       <c r="C626">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D626" t="s">
         <v>3678</v>
@@ -19346,7 +19391,7 @@
         <v>3678</v>
       </c>
     </row>
-    <row r="641" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="641" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A641" t="s">
         <v>786</v>
       </c>
@@ -19354,7 +19399,7 @@
         <v>2515</v>
       </c>
       <c r="C641">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D641" t="s">
         <v>3678</v>
@@ -19385,7 +19430,7 @@
         <v>3678</v>
       </c>
     </row>
-    <row r="644" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="644" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A644" t="s">
         <v>789</v>
       </c>
@@ -19393,7 +19438,7 @@
         <v>2518</v>
       </c>
       <c r="C644">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D644" t="s">
         <v>3678</v>
@@ -19501,7 +19546,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="654" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="654" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A654" t="s">
         <v>799</v>
       </c>
@@ -19509,13 +19554,13 @@
         <v>2528</v>
       </c>
       <c r="C654">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D654" t="s">
         <v>3678</v>
       </c>
     </row>
-    <row r="655" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="655" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A655" t="s">
         <v>800</v>
       </c>
@@ -19523,13 +19568,13 @@
         <v>2529</v>
       </c>
       <c r="C655">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D655" t="s">
         <v>3678</v>
       </c>
     </row>
-    <row r="656" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="656" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A656" t="s">
         <v>801</v>
       </c>
@@ -19537,13 +19582,13 @@
         <v>2530</v>
       </c>
       <c r="C656">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D656" t="s">
         <v>3678</v>
       </c>
     </row>
-    <row r="657" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="657" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A657" t="s">
         <v>802</v>
       </c>
@@ -19551,7 +19596,7 @@
         <v>2531</v>
       </c>
       <c r="C657">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D657" t="s">
         <v>3678</v>
@@ -19758,7 +19803,7 @@
         <v>3678</v>
       </c>
     </row>
-    <row r="676" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="676" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A676" t="s">
         <v>821</v>
       </c>
@@ -19766,13 +19811,13 @@
         <v>2550</v>
       </c>
       <c r="C676">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D676" t="s">
         <v>3678</v>
       </c>
     </row>
-    <row r="677" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="677" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A677" t="s">
         <v>822</v>
       </c>
@@ -19780,7 +19825,7 @@
         <v>2551</v>
       </c>
       <c r="C677">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D677" t="s">
         <v>3678</v>
@@ -19884,7 +19929,7 @@
         <v>3678</v>
       </c>
     </row>
-    <row r="685" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="685" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A685" t="s">
         <v>830</v>
       </c>
@@ -19892,13 +19937,13 @@
         <v>2559</v>
       </c>
       <c r="C685">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D685" t="s">
         <v>3678</v>
       </c>
     </row>
-    <row r="686" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="686" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A686" t="s">
         <v>831</v>
       </c>
@@ -19906,13 +19951,13 @@
         <v>2560</v>
       </c>
       <c r="C686">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D686" t="s">
         <v>3678</v>
       </c>
     </row>
-    <row r="687" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="687" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A687" t="s">
         <v>832</v>
       </c>
@@ -19920,13 +19965,13 @@
         <v>2561</v>
       </c>
       <c r="C687">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D687" t="s">
         <v>3678</v>
       </c>
     </row>
-    <row r="688" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="688" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A688" t="s">
         <v>833</v>
       </c>
@@ -19934,7 +19979,7 @@
         <v>2562</v>
       </c>
       <c r="C688">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D688" t="s">
         <v>3678</v>
@@ -20010,7 +20055,7 @@
         <v>3678</v>
       </c>
     </row>
-    <row r="694" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="694" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A694" t="s">
         <v>839</v>
       </c>
@@ -20018,13 +20063,13 @@
         <v>2568</v>
       </c>
       <c r="C694">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D694" t="s">
         <v>3678</v>
       </c>
     </row>
-    <row r="695" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="695" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A695" t="s">
         <v>840</v>
       </c>
@@ -20032,13 +20077,13 @@
         <v>2569</v>
       </c>
       <c r="C695">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D695" t="s">
         <v>3678</v>
       </c>
     </row>
-    <row r="696" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="696" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A696" t="s">
         <v>841</v>
       </c>
@@ -20046,13 +20091,13 @@
         <v>2570</v>
       </c>
       <c r="C696">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D696" t="s">
         <v>3678</v>
       </c>
     </row>
-    <row r="697" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="697" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A697" t="s">
         <v>842</v>
       </c>
@@ -20060,7 +20105,7 @@
         <v>2571</v>
       </c>
       <c r="C697">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D697" t="s">
         <v>3678</v>
@@ -20351,7 +20396,7 @@
         <v>3678</v>
       </c>
     </row>
-    <row r="722" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="722" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A722" t="s">
         <v>867</v>
       </c>
@@ -20359,7 +20404,7 @@
         <v>2596</v>
       </c>
       <c r="C722">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D722" t="s">
         <v>3678</v>
@@ -20954,7 +20999,7 @@
         <v>3678</v>
       </c>
     </row>
-    <row r="767" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="767" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A767" t="s">
         <v>912</v>
       </c>
@@ -20962,13 +21007,13 @@
         <v>2641</v>
       </c>
       <c r="C767">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D767" t="s">
         <v>3678</v>
       </c>
     </row>
-    <row r="768" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="768" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A768" t="s">
         <v>913</v>
       </c>
@@ -20976,7 +21021,7 @@
         <v>2642</v>
       </c>
       <c r="C768">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D768" t="s">
         <v>3678</v>
@@ -21074,7 +21119,7 @@
         <v>2649</v>
       </c>
       <c r="C775">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D775" t="s">
         <v>3678</v>
@@ -21088,7 +21133,7 @@
         <v>2650</v>
       </c>
       <c r="C776">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D776" t="s">
         <v>3678</v>
@@ -21760,7 +21805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="837" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="837" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A837" t="s">
         <v>982</v>
       </c>
@@ -21768,13 +21813,13 @@
         <v>2710</v>
       </c>
       <c r="C837">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D837" t="s">
         <v>3678</v>
       </c>
     </row>
-    <row r="838" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="838" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A838" t="s">
         <v>983</v>
       </c>
@@ -21782,13 +21827,13 @@
         <v>2711</v>
       </c>
       <c r="C838">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D838" t="s">
         <v>3678</v>
       </c>
     </row>
-    <row r="839" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="839" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A839" t="s">
         <v>984</v>
       </c>
@@ -21796,13 +21841,13 @@
         <v>2712</v>
       </c>
       <c r="C839">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D839" t="s">
         <v>3678</v>
       </c>
     </row>
-    <row r="840" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="840" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A840" t="s">
         <v>985</v>
       </c>
@@ -21810,7 +21855,7 @@
         <v>2713</v>
       </c>
       <c r="C840">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D840" t="s">
         <v>3678</v>
@@ -31796,7 +31841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1745" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1745" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1745" t="s">
         <v>51</v>
       </c>
@@ -31804,7 +31849,7 @@
         <v>126</v>
       </c>
       <c r="C1745">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D1745" t="s">
         <v>3680</v>
@@ -31843,7 +31888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1749" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1749" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1749" t="s">
         <v>55</v>
       </c>
@@ -31851,13 +31896,13 @@
         <v>130</v>
       </c>
       <c r="C1749">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D1749" t="s">
         <v>3680</v>
       </c>
     </row>
-    <row r="1750" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1750" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1750" t="s">
         <v>56</v>
       </c>
@@ -31865,13 +31910,13 @@
         <v>131</v>
       </c>
       <c r="C1750">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D1750" t="s">
         <v>3680</v>
       </c>
     </row>
-    <row r="1751" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1751" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1751" t="s">
         <v>57</v>
       </c>
@@ -31879,13 +31924,13 @@
         <v>132</v>
       </c>
       <c r="C1751">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D1751" t="s">
         <v>3680</v>
       </c>
     </row>
-    <row r="1752" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1752" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1752" t="s">
         <v>58</v>
       </c>
@@ -31893,7 +31938,7 @@
         <v>133</v>
       </c>
       <c r="C1752">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D1752" t="s">
         <v>3680</v>
@@ -31932,7 +31977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1756" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1756" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1756" t="s">
         <v>62</v>
       </c>
@@ -31940,7 +31985,7 @@
         <v>137</v>
       </c>
       <c r="C1756">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D1756" t="s">
         <v>3680</v>
@@ -31990,7 +32035,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1761" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1761" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1761" t="s">
         <v>67</v>
       </c>
@@ -31998,13 +32043,13 @@
         <v>142</v>
       </c>
       <c r="C1761">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D1761" t="s">
         <v>3680</v>
       </c>
     </row>
-    <row r="1762" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1762" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1762" t="s">
         <v>68</v>
       </c>
@@ -32012,13 +32057,13 @@
         <v>143</v>
       </c>
       <c r="C1762">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D1762" t="s">
         <v>3680</v>
       </c>
     </row>
-    <row r="1763" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1763" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1763" t="s">
         <v>69</v>
       </c>
@@ -32026,7 +32071,7 @@
         <v>144</v>
       </c>
       <c r="C1763">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D1763" t="s">
         <v>3680</v>
@@ -32115,16 +32160,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B56"/>
+  <dimension ref="A1:D56"/>
   <sheetViews>
-    <sheetView zoomScale="107" zoomScaleNormal="107" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView topLeftCell="A8" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.5" customWidth="1"/>
     <col min="2" max="2" width="58.33203125" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -32255,7 +32301,7 @@
         <v>3638</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>3600</v>
       </c>
@@ -32263,7 +32309,7 @@
         <v>3639</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>3601</v>
       </c>
@@ -32271,7 +32317,7 @@
         <v>3640</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>3602</v>
       </c>
@@ -32279,15 +32325,21 @@
         <v>3641</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>3603</v>
       </c>
       <c r="B20" t="s">
         <v>3642</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C20" t="s">
+        <v>3683</v>
+      </c>
+      <c r="D20" t="s">
+        <v>3684</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>3604</v>
       </c>
@@ -32295,7 +32347,7 @@
         <v>3643</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>3605</v>
       </c>
@@ -32303,31 +32355,49 @@
         <v>3644</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>3606</v>
       </c>
       <c r="B23" t="s">
         <v>3645</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C23" t="s">
+        <v>3683</v>
+      </c>
+      <c r="D23" t="s">
+        <v>3684</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>3607</v>
       </c>
       <c r="B24" t="s">
         <v>3646</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C24" t="s">
+        <v>3683</v>
+      </c>
+      <c r="D24" t="s">
+        <v>3684</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>3608</v>
       </c>
       <c r="B25" t="s">
         <v>3647</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C25" t="s">
+        <v>3683</v>
+      </c>
+      <c r="D25" t="s">
+        <v>3684</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>3609</v>
       </c>
@@ -32335,7 +32405,7 @@
         <v>3648</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>3610</v>
       </c>
@@ -32343,23 +32413,35 @@
         <v>3649</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>3611</v>
       </c>
       <c r="B28" t="s">
         <v>3650</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C28" t="s">
+        <v>3683</v>
+      </c>
+      <c r="D28" t="s">
+        <v>3684</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>3612</v>
       </c>
       <c r="B29" t="s">
         <v>3651</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C29" t="s">
+        <v>3683</v>
+      </c>
+      <c r="D29" t="s">
+        <v>3684</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>3613</v>
       </c>
@@ -32367,7 +32449,7 @@
         <v>3652</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>3614</v>
       </c>
@@ -32375,7 +32457,7 @@
         <v>3653</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>3615</v>
       </c>
@@ -32582,10 +32664,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:B77"/>
+  <dimension ref="A1:D77"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="B84" sqref="B84"/>
+    <sheetView zoomScale="142" zoomScaleNormal="142" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -32722,7 +32804,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -32730,7 +32812,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -32738,7 +32820,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -32746,7 +32828,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -32754,7 +32836,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -32762,7 +32844,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -32770,7 +32852,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -32778,7 +32860,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -32786,7 +32868,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -32794,7 +32876,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -32802,23 +32884,32 @@
         <v>99</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>25</v>
       </c>
       <c r="B27" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C27" t="s">
+        <v>3683</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>26</v>
       </c>
       <c r="B28" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C28" t="s">
+        <v>3683</v>
+      </c>
+      <c r="D28" t="s">
+        <v>3685</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -32826,15 +32917,21 @@
         <v>102</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>28</v>
       </c>
       <c r="B30" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C30" t="s">
+        <v>3683</v>
+      </c>
+      <c r="D30" t="s">
+        <v>3684</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -32842,7 +32939,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -33217,10 +33314,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView zoomScale="183" zoomScaleNormal="183" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -33357,7 +33454,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>68</v>
       </c>
@@ -33365,7 +33462,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>69</v>
       </c>
@@ -33373,15 +33470,21 @@
         <v>144</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>70</v>
       </c>
       <c r="B19" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C19" t="s">
+        <v>3683</v>
+      </c>
+      <c r="D19" t="s">
+        <v>3686</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>71</v>
       </c>
@@ -33389,7 +33492,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>5</v>
       </c>
@@ -33397,7 +33500,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>3</v>
       </c>

</xml_diff>